<commit_message>
added 5 Negative Login Tests Scenarios using DataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/dataProviders/testData/TestDataProvider.xlsx
+++ b/src/test/resources/dataProviders/testData/TestDataProvider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19163\seleniumArchitecture\QDPM\src\test\resources\dataProviders\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60DD126-0F33-47D4-8F9A-C71BBA5ED6A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71F48C6-F92C-44F5-A1CF-F62630446BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5F7D3B99-D034-441B-B1F7-06ED4F3CD305}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>Sr No</t>
   </si>
@@ -143,9 +143,6 @@
     <t>wrongpassword</t>
   </si>
   <si>
-    <t>wrongusername</t>
-  </si>
-  <si>
     <t>administrator</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>No</t>
   </si>
   <si>
-    <t xml:space="preserve"> No match for Email and/or Password</t>
-  </si>
-  <si>
     <t>Wrong Username + Correct Password</t>
   </si>
   <si>
@@ -177,6 +171,21 @@
   </si>
   <si>
     <t>Wrong Username + Wrong Password</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>credentials</t>
+  </si>
+  <si>
+    <t>fieldRequired</t>
+  </si>
+  <si>
+    <t>wrong@username.com</t>
+  </si>
+  <si>
+    <t>Error: No match for Email and/or Password</t>
   </si>
 </sst>
 </file>
@@ -755,23 +764,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0494A8FF-4968-4880-9D03-3DFBEECE22D0}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>35</v>
@@ -780,13 +789,16 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -797,58 +809,73 @@
         <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>38</v>
+      <c r="B4" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
       </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -856,16 +883,21 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
         <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{E350DC01-921C-4786-8027-CE1FF97FE036}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{75188468-4D0B-402B-A10D-4BF8ECD9D8C1}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{8D97FA5B-D849-4463-9344-56AC8E884A05}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{C94DA276-D314-4478-B352-EAFAB5A22495}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new end to end test 'AddNewUserTest'
</commit_message>
<xml_diff>
--- a/src/test/resources/dataProviders/testData/TestDataProvider.xlsx
+++ b/src/test/resources/dataProviders/testData/TestDataProvider.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19163\seleniumArchitecture\QDPM\src\test\resources\dataProviders\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19163\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71F48C6-F92C-44F5-A1CF-F62630446BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C0987E-29E6-446F-A5E8-163E25225583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5F7D3B99-D034-441B-B1F7-06ED4F3CD305}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskCreationData" sheetId="1" r:id="rId1"/>
-    <sheet name="NegativeLoginTest" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="NegativeLoginTest" sheetId="2" r:id="rId2"/>
+    <sheet name="AddUserData" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
   <si>
     <t>Sr No</t>
   </si>
@@ -35,6 +35,9 @@
     <t>Test Case Name</t>
   </si>
   <si>
+    <t>FullName</t>
+  </si>
+  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
     <t>Label</t>
   </si>
   <si>
+    <t>AssignTo</t>
+  </si>
+  <si>
     <t>StartDate</t>
   </si>
   <si>
@@ -71,96 +77,105 @@
     <t>AttachmentFilePath</t>
   </si>
   <si>
-    <t>CreateTask with Open Status</t>
-  </si>
-  <si>
-    <t>Create Defect wtith Reopen Status</t>
+    <t>Test Project 1</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>administrator@localhost.com</t>
+  </si>
+  <si>
+    <t>administrator</t>
   </si>
   <si>
     <t>Change Priority Rate (Hourly rate $25.00)</t>
   </si>
   <si>
+    <t>dev1</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Medum</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>G:\1. My Cources\Test Case.docx</t>
+  </si>
+  <si>
+    <t>Test Project 2</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>developer@localhost.com</t>
+  </si>
+  <si>
     <t>Defects (Hourly rate $0.00)</t>
   </si>
   <si>
-    <t>Open</t>
+    <t>dev2</t>
   </si>
   <si>
     <t>Re-opened</t>
   </si>
   <si>
-    <t>Task</t>
+    <t>Urgent</t>
   </si>
   <si>
     <t>Bug</t>
   </si>
   <si>
-    <t>Urgent</t>
-  </si>
-  <si>
-    <t>2020-09-28</t>
-  </si>
-  <si>
-    <t>2020-09-29</t>
-  </si>
-  <si>
-    <t>2020-09-30</t>
-  </si>
-  <si>
-    <t>G:\1. My Cources\Test Case.docx</t>
-  </si>
-  <si>
-    <t>dev1</t>
-  </si>
-  <si>
-    <t>dev2</t>
-  </si>
-  <si>
-    <t>Medum</t>
-  </si>
-  <si>
-    <t>FullName</t>
-  </si>
-  <si>
-    <t>developer@localhost.com</t>
-  </si>
-  <si>
-    <t>developer</t>
-  </si>
-  <si>
-    <t>Test Project 1</t>
-  </si>
-  <si>
-    <t>Test Project 2</t>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>Username</t>
   </si>
   <si>
-    <t>administrator@localhost.com</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Expected message</t>
+  </si>
+  <si>
+    <t>info</t>
   </si>
   <si>
     <t>wrongpassword</t>
   </si>
   <si>
-    <t>administrator</t>
-  </si>
-  <si>
-    <t>info</t>
+    <t>credentials</t>
+  </si>
+  <si>
+    <t>Error: No match for Email and/or Password</t>
   </si>
   <si>
     <t>Corret Username + Wrong Password</t>
   </si>
   <si>
-    <t>Expected message</t>
-  </si>
-  <si>
-    <t>No</t>
+    <t>wrong@username.com</t>
   </si>
   <si>
     <t>Wrong Username + Correct Password</t>
   </si>
   <si>
+    <t>Wrong Username + Wrong Password</t>
+  </si>
+  <si>
+    <t>fieldRequired</t>
+  </si>
+  <si>
     <t>This field is required!</t>
   </si>
   <si>
@@ -170,29 +185,122 @@
     <t>Correct Username + Blank Password</t>
   </si>
   <si>
-    <t>Wrong Username + Wrong Password</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>credentials</t>
-  </si>
-  <si>
-    <t>fieldRequired</t>
-  </si>
-  <si>
-    <t>wrong@username.com</t>
-  </si>
-  <si>
-    <t>Error: No match for Email and/or Password</t>
+    <t>LoginEmail</t>
+  </si>
+  <si>
+    <t>LoginPassword</t>
+  </si>
+  <si>
+    <t>AccountUserName</t>
+  </si>
+  <si>
+    <t>ActiveUser</t>
+  </si>
+  <si>
+    <t>UserGroup</t>
+  </si>
+  <si>
+    <t>AcountName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>UserNotify</t>
+  </si>
+  <si>
+    <t>Bruce Willis</t>
+  </si>
+  <si>
+    <t>Bruce</t>
+  </si>
+  <si>
+    <t>bruce@willis.com</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>Quentin Tarantino</t>
+  </si>
+  <si>
+    <t>Quentin</t>
+  </si>
+  <si>
+    <t>quentin@tarantino.com</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>John Travolta</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>john@travolta.com</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>Uma Thurman</t>
+  </si>
+  <si>
+    <t>Uma</t>
+  </si>
+  <si>
+    <t>uma@thurman.com</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Samuel Jackson</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>samuel@jackson.com</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Estimated Time</t>
+  </si>
+  <si>
+    <t>manager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,53 +308,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -258,22 +326,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -306,7 +368,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -318,7 +380,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -365,23 +427,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -417,23 +462,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -585,274 +613,289 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3FA0CC-B4DB-4341-A9AD-E7F79838C2AC}">
-  <dimension ref="A1:O3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="M1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="5">
+      <c r="L2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1">
+        <v>44086</v>
+      </c>
+      <c r="O2" s="1">
+        <v>44103</v>
+      </c>
+      <c r="P2" s="2">
         <v>0.05</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="5">
+      <c r="M3">
+        <v>20</v>
+      </c>
+      <c r="N3" s="1">
+        <v>44084</v>
+      </c>
+      <c r="O3" s="1">
+        <v>44104</v>
+      </c>
+      <c r="P3" s="2">
         <v>0.95</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="admin@123" xr:uid="{DA892068-319F-4704-AFD7-85DEF9591529}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{C8CB71C3-26B2-40D7-961C-59E9144BB3D4}"/>
-    <hyperlink ref="E3" r:id="rId3" display="admin@123" xr:uid="{C564C3E5-8F19-41C7-AEC2-2025A770C8A3}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{9DF2BDC5-5233-40EA-A4B6-887EA488EE09}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0494A8FF-4968-4880-9D03-3DFBEECE22D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C75232-575E-4A02-A1E7-48B5BDCD8DCC}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>36</v>
+      <c r="B2" t="s">
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>51</v>
+      <c r="B3" t="s">
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>51</v>
+      <c r="B4" t="s">
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
         <v>47</v>
@@ -863,54 +906,293 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
         <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>36</v>
+      <c r="B6" t="s">
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{E350DC01-921C-4786-8027-CE1FF97FE036}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{75188468-4D0B-402B-A10D-4BF8ECD9D8C1}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{8D97FA5B-D849-4463-9344-56AC8E884A05}"/>
-    <hyperlink ref="B4" r:id="rId4" xr:uid="{C94DA276-D314-4478-B352-EAFAB5A22495}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C79390A-120B-4E49-82B1-9614284D36BB}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD471D94-BB35-40AB-9296-F3183E49C0F2}">
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="3">
+        <v>9156479854</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="3">
+        <v>9163542158</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="3">
+        <v>9196587412</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="3">
+        <v>9156569874</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" s="3">
+        <v>9154632221</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>